<commit_message>
criado funcao de verificar pedidos em atrasos
</commit_message>
<xml_diff>
--- a/planilha_rota_entregas.xlsx
+++ b/planilha_rota_entregas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>notaFiscal</t>
   </si>
@@ -520,9 +520,7 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>